<commit_message>
updates to glyphlist and cheatsheet
</commit_message>
<xml_diff>
--- a/alists/EpiDoc.xlsx
+++ b/alists/EpiDoc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="262">
   <si>
     <t>K-P</t>
   </si>
@@ -636,19 +636,10 @@
     <t>Symbols, interpuncts, etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">((hedera))  </t>
-  </si>
-  <si>
-    <t>((chi-rho))</t>
-  </si>
-  <si>
     <t>((staurogram)</t>
   </si>
   <si>
     <t>a · b</t>
-  </si>
-  <si>
-    <t>&lt;g type=”chi-rho”/&gt;</t>
   </si>
   <si>
     <t>&lt;g type=”staurogram/&gt;</t>
@@ -805,9 +796,6 @@
     </r>
   </si>
   <si>
-    <t>&lt;g type="hedera"/&gt; now should be &lt;g ref=""&gt; etc.</t>
-  </si>
-  <si>
     <t>Numeral in words?</t>
   </si>
   <si>
@@ -821,6 +809,39 @@
   </si>
   <si>
     <t>U+2766 ❦ floral heart Where unicode symbols exist, these could be used?</t>
+  </si>
+  <si>
+    <t>((corona))</t>
+  </si>
+  <si>
+    <t>&lt;g type="corona"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;g type="hedera"/&gt; 
+&lt;g ref="http://sicily.classics.ox.ac.uk/alists/listglyph.xml#leaf"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">((hedera))
+❦  </t>
+  </si>
+  <si>
+    <t>&lt;g type=”chi-rho”/&gt;
+&lt;g ref="http://sicily.classics.ox.ac.uk/alists/listglyph.xml#chi-rho"/&gt;</t>
+  </si>
+  <si>
+    <t>((chi-rho))
+☧</t>
+  </si>
+  <si>
+    <t xml:space="preserve">((palm branch))
+</t>
+  </si>
+  <si>
+    <t>U+2E19 ⸙</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+&lt;g ref="http://sicily.classics.ox.ac.uk/alists/listglyph.xml#palmbranch"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F85"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1231,7 +1252,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1281,7 +1302,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1426,7 +1447,7 @@
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
@@ -1446,7 +1467,7 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -1474,7 +1495,7 @@
         <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
@@ -1538,7 +1559,7 @@
         <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
@@ -1554,7 +1575,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1674,14 +1695,14 @@
         <v>105</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1742,7 +1763,7 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -1758,7 +1779,7 @@
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -1802,7 +1823,7 @@
         <v>132</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
@@ -1825,7 +1846,7 @@
         <v>136</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1930,7 +1951,7 @@
         <v>160</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
@@ -1950,7 +1971,7 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F47" s="1"/>
     </row>
@@ -1967,7 +1988,7 @@
         <v>167</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1975,7 +1996,7 @@
         <v>168</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>169</v>
@@ -1994,7 +2015,7 @@
         <v>172</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
@@ -2006,7 +2027,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
@@ -2018,7 +2039,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
@@ -2034,7 +2055,7 @@
         <v>177</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
@@ -2068,7 +2089,7 @@
         <v>184</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
@@ -2086,14 +2107,14 @@
         <v>187</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
         <v>191</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2196,7 +2217,7 @@
     <row r="64" spans="1:6">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -2205,7 +2226,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" ht="30">
       <c r="A65" s="1" t="s">
         <v>45</v>
       </c>
@@ -2213,146 +2234,156 @@
         <v>205</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>206</v>
+        <v>256</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="30">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1" t="s">
-        <v>207</v>
+        <v>259</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
-        <v>210</v>
+        <v>261</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="30">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1" t="s">
-        <v>208</v>
+        <v>258</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1" t="s">
-        <v>253</v>
+        <v>206</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F68" t="s">
-        <v>254</v>
+        <v>208</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>209</v>
+        <v>253</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>214</v>
+        <v>249</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>216</v>
+        <v>251</v>
+      </c>
+      <c r="F70" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="71" spans="1:6">
-      <c r="A71" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>216</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="C73" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
+      <c r="E73" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="E74" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
+      <c r="C75" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -2436,6 +2467,22 @@
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ISic0637 etc., Greek inscriptions from Syracuse
Greek inscriptions from Syracuse plus a heart symbol added to the glyph list
</commit_message>
<xml_diff>
--- a/alists/EpiDoc.xlsx
+++ b/alists/EpiDoc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="265">
   <si>
     <t>K-P</t>
   </si>
@@ -843,12 +843,22 @@
     <t xml:space="preserve">
 &lt;g ref="http://sicily.classics.ox.ac.uk/alists/listglyph.xml#palmbranch"/&gt;</t>
   </si>
+  <si>
+    <t>&lt;g ref="http://sicily.classics.ox.ac.uk/alists/listglyph.xml#heart"/&gt;</t>
+  </si>
+  <si>
+    <t>U+2665 ♥</t>
+  </si>
+  <si>
+    <t>((heart))
+♥</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -868,6 +878,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Brill"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -891,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -902,6 +918,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1203,10 +1223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2162,239 +2182,245 @@
       <c r="D60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:6" ht="16.5">
+      <c r="A61" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1" t="s">
+      <c r="D61" s="4"/>
+      <c r="E61" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="1" t="s">
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:6" ht="16.5">
+      <c r="A62" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1" t="s">
+      <c r="C62" s="4"/>
+      <c r="D62" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F62" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:6" ht="16.5">
+      <c r="A63" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1" t="s">
+      <c r="C63" s="4"/>
+      <c r="D63" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1" t="s">
+    <row r="64" spans="1:6" ht="16.5">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1" t="s">
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="30">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:6" ht="33">
+      <c r="A65" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1" t="s">
+      <c r="D65" s="4"/>
+      <c r="E65" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" s="4" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="30">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1" t="s">
+    <row r="66" spans="1:6" ht="33">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="33">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1" t="s">
+      <c r="D67" s="4"/>
+      <c r="E67" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F67" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="30">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1" t="s">
+    <row r="68" spans="1:6" ht="33">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1" t="s">
+      <c r="D68" s="4"/>
+      <c r="E68" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F68" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1" t="s">
+    <row r="69" spans="1:6" ht="16.5">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1" t="s">
+      <c r="D69" s="4"/>
+      <c r="E69" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F69" s="4" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1" t="s">
+    <row r="70" spans="1:6" ht="16.5">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1" t="s">
+      <c r="D70" s="4"/>
+      <c r="E70" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1" t="s">
+      <c r="F70" s="4"/>
+    </row>
+    <row r="71" spans="1:6" ht="16.5">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1" t="s">
+      <c r="D71" s="4"/>
+      <c r="E71" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F71" s="5" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1" t="s">
+    <row r="72" spans="1:6" ht="16.5">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1" t="s">
+      <c r="D72" s="4"/>
+      <c r="E72" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="1" t="s">
+      <c r="F72" s="4"/>
+    </row>
+    <row r="73" spans="1:6" ht="16.5">
+      <c r="A73" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B73" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1" t="s">
+      <c r="D73" s="4"/>
+      <c r="E73" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F73" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="1" t="s">
+    <row r="74" spans="1:6" ht="16.5">
+      <c r="A74" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C74" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1" t="s">
+      <c r="D74" s="4"/>
+      <c r="E74" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F74" s="4" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:6" ht="33">
+      <c r="A75" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C75" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1" t="s">
+      <c r="D75" s="4"/>
+      <c r="E75" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F75" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1" t="s">
+    <row r="76" spans="1:6" ht="16.5">
+      <c r="A76" s="4"/>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="1"/>
@@ -2483,6 +2509,14 @@
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="1"/>
+      <c r="F88" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minor edits and creation of a new file
editing of epidoc of 1574, while 4379 is new file for newly published inscription; minor amendment to epidoc cheatsheet re text direction; trivial edit of 0613.
</commit_message>
<xml_diff>
--- a/alists/EpiDoc.xlsx
+++ b/alists/EpiDoc.xlsx
@@ -589,21 +589,6 @@
   </si>
   <si>
     <t>↺</t>
-  </si>
-  <si>
-    <t>&lt;lb n="1" rend="right-to-left"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;lb n=”1” rend=”left-to-right”/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;lb n=”1” rend=”spiral-clockwise”/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;lb n=”1” rend=”spiral-anticlockwise”/&gt;</t>
-  </si>
-  <si>
-    <t>NB EpiDoc guidelines have changed for this</t>
   </si>
   <si>
     <t>Numeral</t>
@@ -853,12 +838,27 @@
     <t>((heart))
 ♥</t>
   </si>
+  <si>
+    <t>&lt;lb n="1" style="text-direction:r-to-l"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;lb n=”1” style="text-direction:l-to-r”/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;lb n=”1” style="text-direction:clockwise”/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;lb n=”1” style="text-direction:spiral-anticlockwise”/&gt;</t>
+  </si>
+  <si>
+    <t>NB revised epidoc guidelines</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1225,11 +1225,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="100.42578125" bestFit="1" customWidth="1"/>
@@ -1239,7 +1239,7 @@
     <col min="6" max="6" width="255.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1272,10 +1272,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1291,7 +1291,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>13</v>
@@ -1307,7 +1307,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1322,10 +1322,10 @@
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>20</v>
@@ -1341,7 +1341,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
@@ -1443,7 +1443,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>49</v>
       </c>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -1487,11 +1487,11 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>63</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>65</v>
@@ -1539,7 +1539,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="30">
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>80</v>
@@ -1595,11 +1595,11 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>81</v>
       </c>
@@ -1615,7 +1615,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>81</v>
       </c>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>90</v>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>93</v>
@@ -1675,7 +1675,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>97</v>
       </c>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>101</v>
       </c>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>101</v>
       </c>
@@ -1715,17 +1715,17 @@
         <v>105</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>107</v>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>110</v>
       </c>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>114</v>
       </c>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" ht="30">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>118</v>
       </c>
@@ -1783,11 +1783,11 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>118</v>
       </c>
@@ -1799,11 +1799,11 @@
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>123</v>
       </c>
@@ -1819,7 +1819,7 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>127</v>
       </c>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>131</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>132</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
@@ -1853,7 +1853,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="30">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>135</v>
@@ -1866,10 +1866,10 @@
         <v>136</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>137</v>
       </c>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>141</v>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>144</v>
@@ -1915,7 +1915,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>148</v>
       </c>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>152</v>
       </c>
@@ -1947,7 +1947,7 @@
       </c>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>156</v>
@@ -1963,7 +1963,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>159</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>160</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="1:6" ht="30">
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>162</v>
       </c>
@@ -1991,11 +1991,11 @@
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" ht="30">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
         <v>165</v>
@@ -2008,15 +2008,15 @@
         <v>167</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>169</v>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>171</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>172</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
@@ -2043,11 +2043,11 @@
       </c>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
@@ -2055,11 +2055,11 @@
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
@@ -2067,7 +2067,7 @@
       </c>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>176</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>177</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>179</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>45</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>184</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
@@ -2119,7 +2119,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>45</v>
       </c>
@@ -2127,17 +2127,17 @@
         <v>187</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>191</v>
+        <v>260</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
@@ -2145,13 +2145,13 @@
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>192</v>
+        <v>261</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
@@ -2159,11 +2159,11 @@
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>193</v>
+        <v>262</v>
       </c>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
@@ -2171,258 +2171,258 @@
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>194</v>
+        <v>263</v>
       </c>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6" ht="16.5">
+    <row r="61" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" spans="1:6" ht="16.5">
+    <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="16.5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="16.5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A64" s="4"/>
       <c r="B64" s="4" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="F64" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="33">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="33">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="4"/>
       <c r="C66" s="4" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="33">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="33">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="16.5">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="16.5">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" spans="1:6" ht="16.5">
+    <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="16.5">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" spans="1:6" ht="16.5">
+    <row r="73" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="16.5">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="33">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="16.5">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A76" s="4"/>
       <c r="B76" s="4"/>
       <c r="C76" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2430,7 +2430,7 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2438,7 +2438,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2446,7 +2446,7 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2454,7 +2454,7 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2462,7 +2462,7 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2470,7 +2470,7 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2478,7 +2478,7 @@
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2486,7 +2486,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2494,7 +2494,7 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2502,7 +2502,7 @@
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2510,7 +2510,7 @@
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2530,7 +2530,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2542,7 +2542,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
checking and approving text div edits
Work by Alex Antoniou, Tom Gavin, Sinja Kuppers
</commit_message>
<xml_diff>
--- a/alists/EpiDoc.xlsx
+++ b/alists/EpiDoc.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corp1223\Documents\GitHub\ISicily\alists\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA41D922-25EA-447E-85C0-A8A00185085C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="269">
   <si>
     <t>K-P</t>
   </si>
@@ -712,9 +706,6 @@
   </si>
   <si>
     <t>U+2627 ☧ Chi Rho</t>
-  </si>
-  <si>
-    <t>Can be nested with other text divs; must be followed by &lt;ab&gt;. Not necessary except when fragments are discrete and do not join?</t>
   </si>
   <si>
     <t>For main display of individual inscription, use line-break for new line; use / for display of text e.g. in griddisplay of search results, etc. If possible, line numbers should be displayed in the margin at e.g. 5 line intervals.</t>
@@ -859,12 +850,27 @@
   <si>
     <t>r</t>
   </si>
+  <si>
+    <t>Text on separate surfaces of stone</t>
+  </si>
+  <si>
+    <t>Face (a)</t>
+  </si>
+  <si>
+    <t>&lt;div type="textpart" subtype="face" n="a"&gt;</t>
+  </si>
+  <si>
+    <t>Nest within &lt;div type="edition"&gt;; must be followed by &lt;ab&gt;. Not necessary except when fragments are discrete and do not join?</t>
+  </si>
+  <si>
+    <t>Nest within &lt;div type="edition"&gt;; must be followed by &lt;ab&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,7 +1016,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1043,26 +1049,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1095,23 +1084,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1287,14 +1259,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F88"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="100.42578125" bestFit="1" customWidth="1"/>
@@ -1304,7 +1276,7 @@
     <col min="6" max="6" width="255.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1324,7 +1296,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -1337,10 +1309,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1353,935 +1325,933 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>264</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>265</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C12" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>216</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>58</v>
+        <v>216</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>217</v>
+        <v>55</v>
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>217</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" ht="17.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>264</v>
+        <v>60</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1"/>
+    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>263</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6">
+        <v>67</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>218</v>
+        <v>75</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="30">
-      <c r="A22" s="1"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>232</v>
+        <v>79</v>
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="1" t="s">
-        <v>81</v>
-      </c>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>83</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>84</v>
+        <v>231</v>
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="1"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="B26" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6">
+        <v>95</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>233</v>
+        <v>103</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="B31" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>108</v>
+        <v>232</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1" t="s">
-        <v>110</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" ht="30">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>234</v>
+        <v>117</v>
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" ht="30">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>126</v>
+        <v>234</v>
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>220</v>
+        <v>129</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30">
-      <c r="A39" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="B39" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>26</v>
+        <v>220</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="1" t="s">
-        <v>137</v>
-      </c>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="B41" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" s="1" t="s">
-        <v>148</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6">
+        <v>146</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6">
-      <c r="A45" s="1"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="B45" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>154</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
-      <c r="A46" s="1" t="s">
-        <v>159</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>221</v>
+        <v>154</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" ht="30">
+        <v>157</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>164</v>
+        <v>221</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>237</v>
+        <v>161</v>
       </c>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="1:6" ht="30">
-      <c r="A48" s="1"/>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="B48" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>222</v>
+        <v>165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6">
+        <v>167</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="C51" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>177</v>
-      </c>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>181</v>
+        <v>226</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+        <v>178</v>
+      </c>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>239</v>
+        <v>181</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>258</v>
+        <v>185</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="C57" s="1" t="s">
-        <v>188</v>
+        <v>239</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6">
+        <v>258</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D60" s="1"/>
+      <c r="E60" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:6" ht="16.5">
-      <c r="A61" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F61" s="4"/>
-    </row>
-    <row r="62" spans="1:6" ht="16.5">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4" t="s">
-        <v>194</v>
-      </c>
+      <c r="C62" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D62" s="4"/>
       <c r="E62" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="16.5">
+        <v>193</v>
+      </c>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>45</v>
       </c>
@@ -2290,74 +2260,78 @@
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="16.5">
-      <c r="A64" s="4"/>
+    <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="B64" s="4" t="s">
-        <v>241</v>
+        <v>191</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
+      <c r="D64" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>198</v>
+      </c>
       <c r="F64" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="33">
-      <c r="A65" s="4" t="s">
+    <row r="66" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B66" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C65" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4" t="s">
+      <c r="C66" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="33">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4" t="s">
-        <v>257</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="33">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="4"/>
       <c r="C67" s="4" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
         <v>254</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="33">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4" t="s">
@@ -2365,137 +2339,143 @@
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="16.5">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
-        <v>201</v>
+        <v>250</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="16.5">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F70" s="4"/>
-    </row>
-    <row r="71" spans="1:6" ht="16.5">
+        <v>203</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="16.5">
+        <v>246</v>
+      </c>
+      <c r="F71" s="4"/>
+    </row>
+    <row r="72" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="F72" s="4"/>
-    </row>
-    <row r="73" spans="1:6" ht="16.5">
-      <c r="A73" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>204</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
       <c r="C73" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="16.5">
+        <v>228</v>
+      </c>
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F74" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="33">
+    <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="F75" s="4" t="s">
+      <c r="F76" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="16.5">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4" t="s">
+    <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2503,7 +2483,7 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2511,7 +2491,7 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2519,7 +2499,7 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2527,7 +2507,7 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2535,7 +2515,7 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2543,7 +2523,7 @@
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2551,7 +2531,7 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2559,7 +2539,7 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2567,7 +2547,7 @@
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2575,13 +2555,21 @@
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="F89" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2590,24 +2578,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
editing files for Halaesa
based on 2017 edition / autopsy
</commit_message>
<xml_diff>
--- a/alists/EpiDoc.xlsx
+++ b/alists/EpiDoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="275">
   <si>
     <t>K-P</t>
   </si>
@@ -876,6 +876,12 @@
   </si>
   <si>
     <t>use English for the annotation, not Latin</t>
+  </si>
+  <si>
+    <t>Letters one above the other</t>
+  </si>
+  <si>
+    <t>&lt;hi rend="stacked"&gt;to&lt;/hi&gt;</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,92 +1597,90 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>273</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>218</v>
+        <v>75</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>218</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>231</v>
+        <v>79</v>
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>81</v>
-      </c>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>83</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>84</v>
+        <v>231</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -1685,106 +1689,106 @@
         <v>81</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>269</v>
+        <v>93</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>270</v>
+        <v>94</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>271</v>
+        <v>95</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>98</v>
+        <v>269</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>99</v>
+        <v>270</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F30" s="1"/>
+        <v>271</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -1793,78 +1797,78 @@
         <v>101</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>232</v>
+        <v>103</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>219</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="B33" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>108</v>
+        <v>232</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>233</v>
+        <v>117</v>
       </c>
       <c r="F36" s="1"/>
     </row>
@@ -1873,266 +1877,270 @@
         <v>118</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>126</v>
+        <v>234</v>
       </c>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>220</v>
+        <v>129</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="B41" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>26</v>
+        <v>220</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>137</v>
-      </c>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="B43" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>147</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F45" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="B47" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>154</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>158</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>159</v>
-      </c>
+      <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>221</v>
+        <v>154</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>164</v>
+        <v>221</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>236</v>
+        <v>161</v>
       </c>
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="B50" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
-        <v>222</v>
+        <v>165</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="F51" s="1"/>
+        <v>167</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>223</v>
+        <v>169</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>172</v>
+      </c>
       <c r="C53" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F53" s="1"/>
     </row>
@@ -2140,144 +2148,140 @@
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>177</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
       <c r="C55" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>181</v>
+        <v>226</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>183</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>238</v>
+        <v>181</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1" t="s">
-        <v>257</v>
+        <v>185</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="C59" s="1" t="s">
-        <v>188</v>
+        <v>239</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>258</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="D62" s="1"/>
+      <c r="E62" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F63" s="4"/>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
@@ -2286,16 +2290,14 @@
       <c r="B64" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4" t="s">
-        <v>194</v>
-      </c>
+      <c r="C64" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>196</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="F64" s="4"/>
     </row>
     <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
@@ -2306,210 +2308,220 @@
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
+      <c r="A66" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="B66" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4" t="s">
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
+    <row r="68" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A69" s="4"/>
       <c r="B69" s="4"/>
       <c r="C69" s="4" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A70" s="4"/>
       <c r="B70" s="4"/>
       <c r="C70" s="4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A71" s="4"/>
       <c r="B71" s="4"/>
       <c r="C71" s="4" t="s">
-        <v>201</v>
+        <v>250</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>262</v>
+        <v>229</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A72" s="4"/>
       <c r="B72" s="4"/>
       <c r="C72" s="4" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="F72" s="4"/>
+        <v>203</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="73" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A73" s="4"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>242</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A74" s="4"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="F74" s="4"/>
+        <v>243</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>204</v>
-      </c>
+      <c r="A75" s="4"/>
+      <c r="B75" s="4"/>
       <c r="C75" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>207</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="F75" s="4"/>
     </row>
     <row r="76" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F76" s="4" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="F77" s="4" t="s">
+      <c r="F78" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4" t="s">
+    <row r="79" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A79" s="4"/>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
@@ -2598,6 +2610,14 @@
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>